<commit_message>
we are updating things for new server design with better pictures
</commit_message>
<xml_diff>
--- a/database/metadata_linux.xlsx
+++ b/database/metadata_linux.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,190 +484,202 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>w3/1hs.xlsx</t>
+          <t>m4/~$Boss.xlsx</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1hs</t>
+          <t>~$Boss</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>w3/2hs.xlsx</t>
+          <t>w3/1hs.xlsx</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2hs</t>
+          <t>1hs</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>w3/Additional.xlsx</t>
+          <t>w3/2hs.xlsx</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Additional</t>
+          <t>2hs</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>w3/Armor.xlsx</t>
+          <t>w3/Additional.xlsx</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Armor</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>w3/Arrow.xlsx</t>
+          <t>w3/Armor.xlsx</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Arrow</t>
+          <t>Armor</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>w3/Bow.xlsx</t>
+          <t>w3/Arrow.xlsx</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Bow</t>
+          <t>Arrow</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>w3/Bowgun.xlsx</t>
+          <t>w3/Bow.xlsx</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bowgun</t>
+          <t>Bow</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>w3/Dagger.xlsx</t>
+          <t>w3/Bowgun.xlsx</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Dagger</t>
+          <t>Bowgun</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>w3/Halberd.xlsx</t>
+          <t>w3/Dagger.xlsx</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Halberd</t>
+          <t>Dagger</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>w3/Katana.xlsx</t>
+          <t>w3/Halberd.xlsx</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Katana</t>
+          <t>Halberd</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>w3/Knuckles.xlsx</t>
+          <t>w3/Katana.xlsx</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Knuckles</t>
+          <t>Katana</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>w3/Magic_Device.xlsx</t>
+          <t>w3/Knuckles.xlsx</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Magic_Device</t>
+          <t>Knuckles</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>w3/Ninjutsu_Scroll.xlsx</t>
+          <t>w3/Magic_Device.xlsx</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ninjutsu_Scroll</t>
+          <t>Magic_Device</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>w3/Shield.xlsx</t>
+          <t>w3/Ninjutsu_Scroll.xlsx</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Shield</t>
+          <t>Ninjutsu_Scroll</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>w3/Special.xlsx</t>
+          <t>w3/Shield.xlsx</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Special</t>
+          <t>Shield</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>w3/Special.xlsx</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Special</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>w3/Staff.xlsx</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>Staff</t>
         </is>

</xml_diff>